<commit_message>
Add copyrights for figures in Chapter 2
</commit_message>
<xml_diff>
--- a/files/correction list.xlsx
+++ b/files/correction list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezhan/work/mywriting/thesis/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE7E231C-0DC9-AA49-81E7-ADEB01048FD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3399E20D-71A1-D64B-84BE-70CD880D65E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{191DB978-43CC-054F-9BCC-FB5D3B62670D}"/>
+    <workbookView xWindow="26580" yWindow="500" windowWidth="24620" windowHeight="28300" xr2:uid="{191DB978-43CC-054F-9BCC-FB5D3B62670D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
   <si>
     <t>Comments</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>2) Chapter 2: Make sure you have permission to include the figures taken from other references</t>
-  </si>
-  <si>
-    <t>3) Chapter 3: Add a section to describe the experimental methodology in detail, including figures of the setup if possible Include a method section to show how you obtained the data and a picture of the experiment.</t>
   </si>
   <si>
     <t>5) Conclusions: Explain how you have addressed the research questions in the thesis and highlight the impact of this work on the field.</t>
@@ -252,6 +249,18 @@
   </si>
   <si>
     <t>Section 6.2 and refered in Acronyms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">obtain permission for any image reproductions such as fig 2.5 This is usually just a matter of applying to the publisher. See https://www.acm.org/publications/policies/copyright-policy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Permissions have been obtain. The copyrights of figures are stated in Figure 2.1, 2.4, 2.5, 2.6, 2.7, 2.8, 2.9 following the rules of publishers. </t>
+  </si>
+  <si>
+    <t>Permissions have been obtain. The copyrights of figures are stated in Figure 2.1, 2.4, 2.5, 2.6, 2.7, 2.8, 2.9 following the rules of publishers (same in comment 2).</t>
+  </si>
+  <si>
+    <t>3) Chapter 3: Add a section to describe the experimental methodology in detail, including figures of the setup if possible. Include a method section to show how you obtained the data and a picture of the experiment.</t>
   </si>
 </sst>
 </file>
@@ -308,7 +317,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -501,11 +510,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -531,6 +553,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -558,14 +589,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -884,7 +913,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -895,247 +924,249 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="43" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11"/>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
+      <c r="A1" s="14"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
     </row>
     <row r="2" spans="1:3" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="15"/>
+      <c r="B2" s="18"/>
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="17"/>
+      <c r="B3" s="20"/>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="4"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="4" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="5" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="22"/>
+    </row>
+    <row r="6" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="10"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="C9" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="15"/>
+      <c r="B12" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="2" t="s">
+      <c r="C12" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="15"/>
+      <c r="B13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="12"/>
-      <c r="B12" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="4" t="s">
+    <row r="14" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="15"/>
+      <c r="B14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="12"/>
-      <c r="B13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="12"/>
-      <c r="B14" s="2" t="s">
+    <row r="15" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="15"/>
+      <c r="B15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="12"/>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="15"/>
+      <c r="B16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="12"/>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="74" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>24</v>
+      <c r="B17" s="23" t="s">
+        <v>46</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C19" s="4"/>
+    </row>
+    <row r="20" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="15"/>
+      <c r="B20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="12" t="s">
+    <row r="21" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="4"/>
-    </row>
-    <row r="20" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="12"/>
-      <c r="B20" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C21" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="16"/>
+      <c r="B22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="13"/>
-      <c r="B22" s="2" t="s">
+    <row r="23" spans="1:3" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="16"/>
+      <c r="B23" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C23" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="16"/>
+      <c r="B24" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="13"/>
-      <c r="B23" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="13"/>
-      <c r="B24" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="C25" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26" s="19"/>
+      <c r="C26" s="10"/>
     </row>
     <row r="27" spans="1:3" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C27" s="20"/>
+      <c r="C27" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>

<commit_message>
Add methodology section in Chapter 3
</commit_message>
<xml_diff>
--- a/files/correction list.xlsx
+++ b/files/correction list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezhan/work/mywriting/thesis/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3399E20D-71A1-D64B-84BE-70CD880D65E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD6836D-538B-ED46-876A-4C07FAD05AC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26580" yWindow="500" windowWidth="24620" windowHeight="28300" xr2:uid="{191DB978-43CC-054F-9BCC-FB5D3B62670D}"/>
+    <workbookView xWindow="10180" yWindow="500" windowWidth="24620" windowHeight="28300" xr2:uid="{191DB978-43CC-054F-9BCC-FB5D3B62670D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
   <si>
     <t>Comments</t>
   </si>
@@ -262,12 +262,18 @@
   <si>
     <t>3) Chapter 3: Add a section to describe the experimental methodology in detail, including figures of the setup if possible. Include a method section to show how you obtained the data and a picture of the experiment.</t>
   </si>
+  <si>
+    <t>To explain this more in Section 3.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add a section. Make a figure of procedures. Include a photo of the setup. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -302,6 +308,13 @@
       <color theme="1"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -527,7 +540,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -562,6 +575,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -589,12 +608,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -912,8 +930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{853A3EC1-90B9-564D-8415-548D56B5B189}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -924,61 +942,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="43" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14"/>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
+      <c r="A1" s="16"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
     </row>
     <row r="2" spans="1:3" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="18"/>
+      <c r="B2" s="20"/>
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="20"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="13"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="4" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="22"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="24" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="4"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="23" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="13"/>
+      <c r="B7" s="15"/>
       <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="13"/>
+      <c r="B8" s="15"/>
       <c r="C8" s="4" t="s">
         <v>34</v>
       </c>
@@ -1006,7 +1028,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="17" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1017,7 +1039,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="15"/>
+      <c r="A12" s="17"/>
       <c r="B12" s="2" t="s">
         <v>37</v>
       </c>
@@ -1026,7 +1048,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="15"/>
+      <c r="A13" s="17"/>
       <c r="B13" s="2" t="s">
         <v>12</v>
       </c>
@@ -1035,7 +1057,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="15"/>
+      <c r="A14" s="17"/>
       <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
@@ -1044,7 +1066,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="15"/>
+      <c r="A15" s="17"/>
       <c r="B15" s="2" t="s">
         <v>14</v>
       </c>
@@ -1053,7 +1075,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="15"/>
+      <c r="A16" s="17"/>
       <c r="B16" s="2" t="s">
         <v>15</v>
       </c>
@@ -1062,10 +1084,10 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="74" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="13" t="s">
         <v>46</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -1084,7 +1106,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="17" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -1093,7 +1115,7 @@
       <c r="C19" s="4"/>
     </row>
     <row r="20" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="15"/>
+      <c r="A20" s="17"/>
       <c r="B20" s="2" t="s">
         <v>22</v>
       </c>
@@ -1102,7 +1124,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -1113,7 +1135,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="16"/>
+      <c r="A22" s="18"/>
       <c r="B22" s="2" t="s">
         <v>24</v>
       </c>
@@ -1122,7 +1144,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="16"/>
+      <c r="A23" s="18"/>
       <c r="B23" s="2" t="s">
         <v>25</v>
       </c>
@@ -1131,7 +1153,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="16"/>
+      <c r="A24" s="18"/>
       <c r="B24" s="2" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Explain forward progress and how it is measured
</commit_message>
<xml_diff>
--- a/files/correction list.xlsx
+++ b/files/correction list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezhan/work/mywriting/thesis/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD6836D-538B-ED46-876A-4C07FAD05AC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C89BE57-478A-A14D-8779-415C425EAD58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10180" yWindow="500" windowWidth="24620" windowHeight="28300" xr2:uid="{191DB978-43CC-054F-9BCC-FB5D3B62670D}"/>
   </bookViews>
@@ -266,14 +266,14 @@
     <t>To explain this more in Section 3.1</t>
   </si>
   <si>
-    <t xml:space="preserve">Add a section. Make a figure of procedures. Include a photo of the setup. </t>
+    <t>Add Section 3.2 and Figure 3.3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -315,6 +315,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -611,8 +616,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">

</xml_diff>

<commit_message>
Move all related work to Chapter 2
</commit_message>
<xml_diff>
--- a/files/correction list.xlsx
+++ b/files/correction list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezhan/work/mywriting/thesis/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CA6036-445B-2144-8D68-3A54445E4382}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34912F4F-6039-2A48-AF55-DECFF23E5701}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10180" yWindow="500" windowWidth="24620" windowHeight="28300" xr2:uid="{191DB978-43CC-054F-9BCC-FB5D3B62670D}"/>
+    <workbookView xWindow="11700" yWindow="500" windowWidth="27340" windowHeight="28300" xr2:uid="{191DB978-43CC-054F-9BCC-FB5D3B62670D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,13 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
-  <si>
-    <t>Comments</t>
-  </si>
-  <si>
-    <t>Corrections</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
   <si>
     <t>1) Add a table for acronyms</t>
   </si>
@@ -170,116 +164,139 @@
 (referred by the PDF page number in the submitted thesis)</t>
   </si>
   <si>
-    <r>
-      <t>See below:
-(page numbered in the revised thesis as &lt;</t>
-    </r>
+    <t>Figure 1.2</t>
+  </si>
+  <si>
+    <t>Section 1.2</t>
+  </si>
+  <si>
+    <t>"as well as their works" not sure what is meant here. Do you mean "as well as the associated research works"? Or perhaps "as well as how they work"?</t>
+  </si>
+  <si>
+    <t>Section 2.4</t>
+  </si>
+  <si>
+    <t>Section 2.4.1</t>
+  </si>
+  <si>
+    <t>Corrected in Section 5.1</t>
+  </si>
+  <si>
+    <t>Updated in Equation 5.1</t>
+  </si>
+  <si>
+    <t>Section 5.2.2.1</t>
+  </si>
+  <si>
+    <t>Section 6.2 and refered in Acronyms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">obtain permission for any image reproductions such as fig 2.5 This is usually just a matter of applying to the publisher. See https://www.acm.org/publications/policies/copyright-policy </t>
+  </si>
+  <si>
+    <t>Permissions have been obtain. The copyrights of figures are stated in Figure 2.1, 2.4, 2.5, 2.6, 2.7, 2.8, 2.9 following the rules of publishers (same in comment 2).</t>
+  </si>
+  <si>
+    <t>3) Chapter 3: Add a section to describe the experimental methodology in detail, including figures of the setup if possible. Include a method section to show how you obtained the data and a picture of the experiment.</t>
+  </si>
+  <si>
+    <t>Done in Chapter 3 intro and experimental setup</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Add Section 6.1 and relate research questions to the corresponding answers</t>
+  </si>
+  <si>
+    <t>Todo</t>
+  </si>
+  <si>
+    <t>This has been corrected and no other occurrence has been found.</t>
+  </si>
+  <si>
+    <t>I believe this description is misleading. The "maximum voltage drop" was intended to decribe the voltage drop in the case that no energy is gained during the operation, while other factors that increase the voltage drop are meant to be excluded in the term here. This has been rephrased in Section 5.</t>
+  </si>
+  <si>
+    <t>Add Section 3.2 and Figure 3.3. 
+I could not find the picture of the experiment in Chapter 3 as it was old and lost. However, a picture of the experiment in Chapter 5 was found, and it is similar to the setup in Chatper 3. I hope this can at least demonstrate what it looks like.</t>
+  </si>
+  <si>
+    <t>See below</t>
+  </si>
+  <si>
     <r>
       <rPr>
-        <i/>
-        <sz val="12"/>
+        <b/>
+        <sz val="18"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>PDF page</t>
+      <t>Comments</t>
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="18"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>&gt; / &lt;</t>
+      <t xml:space="preserve">
+</t>
     </r>
     <r>
       <rPr>
-        <i/>
         <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>(page numbered in the PDF pages of the submitted thesis)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>text page</t>
+      <t>Corrections</t>
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="18"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>&gt;)</t>
+      <t xml:space="preserve">
+</t>
     </r>
-  </si>
-  <si>
-    <t>Figure 1.2</t>
-  </si>
-  <si>
-    <t>Section 1.2</t>
-  </si>
-  <si>
-    <t>"as well as their works" not sure what is meant here. Do you mean "as well as the associated research works"? Or perhaps "as well as how they work"?</t>
-  </si>
-  <si>
-    <t>Section 2.4</t>
-  </si>
-  <si>
-    <t>Section 2.4.1</t>
-  </si>
-  <si>
-    <t>(Review the whole thesis again )</t>
-  </si>
-  <si>
-    <t>I believe this description is misleading. The "maximum voltage drop" was intended to decribe the voltage drop in the case that no energy is gained during the operation. This has been rephrased in Section 5.</t>
-  </si>
-  <si>
-    <t>Corrected in Section 5.1</t>
-  </si>
-  <si>
-    <t>Updated in Equation 5.1</t>
-  </si>
-  <si>
-    <t>Section 5.2.2.1</t>
-  </si>
-  <si>
-    <t>Section 6.2 and refered in Acronyms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">obtain permission for any image reproductions such as fig 2.5 This is usually just a matter of applying to the publisher. See https://www.acm.org/publications/policies/copyright-policy </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Permissions have been obtain. The copyrights of figures are stated in Figure 2.1, 2.4, 2.5, 2.6, 2.7, 2.8, 2.9 following the rules of publishers. </t>
-  </si>
-  <si>
-    <t>Permissions have been obtain. The copyrights of figures are stated in Figure 2.1, 2.4, 2.5, 2.6, 2.7, 2.8, 2.9 following the rules of publishers (same in comment 2).</t>
-  </si>
-  <si>
-    <t>3) Chapter 3: Add a section to describe the experimental methodology in detail, including figures of the setup if possible. Include a method section to show how you obtained the data and a picture of the experiment.</t>
-  </si>
-  <si>
-    <t>Add Section 3.2 and Figure 3.3</t>
-  </si>
-  <si>
-    <t>Done in Chapter 3 intro and experimental setup</t>
-  </si>
-  <si>
-    <t>Done</t>
-  </si>
-  <si>
-    <t>Add Section 6.1 and relate research questions to the corresponding answers</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>(page numbered in the revised thesis as &lt;PDF page&gt; / &lt;content page&gt;)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">All permissions have been obtain. The copyrights of figures are stated in Figure 2.1, 2.4, 2.5, 2.6, 2.7, 2.8, 2.9 following the guidance of publishers. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -326,6 +343,19 @@
       <color theme="1"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -341,7 +371,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -515,21 +545,6 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -564,56 +579,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -627,17 +608,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -953,285 +961,286 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{853A3EC1-90B9-564D-8415-548D56B5B189}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.83203125" customWidth="1"/>
     <col min="2" max="2" width="50.83203125" customWidth="1"/>
-    <col min="3" max="3" width="60.83203125" customWidth="1"/>
+    <col min="3" max="3" width="62.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="43" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-    </row>
-    <row r="2" spans="1:3" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+    <row r="1" spans="1:3" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
+      <c r="B5" s="5"/>
+      <c r="C5" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="4" t="s">
+      <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
+      <c r="B11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4"/>
+      <c r="B12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+      <c r="B13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+      <c r="B14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
+      <c r="B15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="74" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
+      <c r="B19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="18"/>
+      <c r="B21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="18"/>
+      <c r="B22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="18"/>
+      <c r="B23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="22" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="23" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="16"/>
-      <c r="B12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="16"/>
-      <c r="B13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="16"/>
-      <c r="B14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="16"/>
-      <c r="B15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="16"/>
-      <c r="B16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="74" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="4"/>
-    </row>
-    <row r="20" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="16"/>
-      <c r="B20" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="25" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="17"/>
-      <c r="B22" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="17"/>
-      <c r="B23" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="17"/>
-      <c r="B24" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" s="11"/>
-    </row>
-    <row r="27" spans="1:3" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" s="24"/>
-    </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A11:A16"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="A19:A20"/>
+  <mergeCells count="10">
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>